<commit_message>
adding percentages to pieplot
</commit_message>
<xml_diff>
--- a/src/files/STRIGIFORMES.xlsx
+++ b/src/files/STRIGIFORMES.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TCC\Aves de rapina\Tabelas\pizza\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{725D065F-6492-492B-9B17-0AEE8C569F39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" xr2:uid="{8AE05C7D-51CC-4B10-B363-BF727A0A7EE8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="10920"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -31,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="16">
   <si>
     <t>STRIGIFORMES</t>
   </si>
@@ -73,9 +67,6 @@
   </si>
   <si>
     <t>Asio clamator</t>
-  </si>
-  <si>
-    <t>Arame farpado</t>
   </si>
   <si>
     <t>Athene cunicularia</t>
@@ -87,8 +78,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -218,7 +209,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -270,7 +261,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -464,27 +455,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EF5116B-BCA2-4CEB-B6F6-C19B49A4C674}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="B100" sqref="B100"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B77" sqref="B77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23" style="1" customWidth="1"/>
     <col min="2" max="2" width="24.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="18" thickBot="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -492,15 +483,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="15.75" thickTop="1">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -508,7 +499,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -516,7 +507,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
@@ -524,7 +515,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
@@ -532,7 +523,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
@@ -540,7 +531,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" s="3" t="s">
         <v>2</v>
       </c>
@@ -548,15 +539,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2">
       <c r="A9" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
       <c r="A10" s="3" t="s">
         <v>2</v>
       </c>
@@ -564,7 +555,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2">
       <c r="A11" s="3" t="s">
         <v>2</v>
       </c>
@@ -572,7 +563,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2">
       <c r="A12" s="3" t="s">
         <v>2</v>
       </c>
@@ -580,7 +571,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2">
       <c r="A13" s="3" t="s">
         <v>2</v>
       </c>
@@ -588,7 +579,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2">
       <c r="A14" s="3" t="s">
         <v>2</v>
       </c>
@@ -596,7 +587,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2">
       <c r="A15" s="3" t="s">
         <v>2</v>
       </c>
@@ -604,7 +595,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2">
       <c r="A16" s="3" t="s">
         <v>2</v>
       </c>
@@ -612,7 +603,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="A17" s="3" t="s">
         <v>2</v>
       </c>
@@ -620,7 +611,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2">
       <c r="A18" s="3" t="s">
         <v>2</v>
       </c>
@@ -628,7 +619,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2">
       <c r="A19" s="3" t="s">
         <v>2</v>
       </c>
@@ -636,7 +627,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2">
       <c r="A20" s="3" t="s">
         <v>2</v>
       </c>
@@ -644,15 +635,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2">
       <c r="A21" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
       <c r="A22" s="3" t="s">
         <v>2</v>
       </c>
@@ -660,23 +651,23 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2">
       <c r="A23" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
       <c r="A24" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
       <c r="A25" s="3" t="s">
         <v>2</v>
       </c>
@@ -684,7 +675,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2">
       <c r="A26" s="3" t="s">
         <v>2</v>
       </c>
@@ -692,15 +683,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2">
       <c r="A27" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
       <c r="A28" s="3" t="s">
         <v>2</v>
       </c>
@@ -708,63 +699,63 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2">
       <c r="A29" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
       <c r="A30" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
       <c r="A31" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
       <c r="A32" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
       <c r="A33" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
       <c r="A34" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
       <c r="A35" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
       <c r="A36" s="3" t="s">
         <v>2</v>
       </c>
@@ -772,7 +763,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2">
       <c r="A37" s="3" t="s">
         <v>2</v>
       </c>
@@ -780,7 +771,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2">
       <c r="A38" s="4" t="s">
         <v>10</v>
       </c>
@@ -788,7 +779,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2">
       <c r="A39" s="4" t="s">
         <v>10</v>
       </c>
@@ -796,15 +787,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2">
       <c r="A40" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
       <c r="A41" s="4" t="s">
         <v>10</v>
       </c>
@@ -812,7 +803,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2">
       <c r="A42" s="4" t="s">
         <v>10</v>
       </c>
@@ -820,7 +811,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2">
       <c r="A43" s="4" t="s">
         <v>10</v>
       </c>
@@ -828,7 +819,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2">
       <c r="A44" s="4" t="s">
         <v>10</v>
       </c>
@@ -836,39 +827,39 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2">
       <c r="A45" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
       <c r="A46" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
       <c r="A47" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
       <c r="A48" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
       <c r="A49" s="4" t="s">
         <v>10</v>
       </c>
@@ -876,7 +867,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2">
       <c r="A50" s="4" t="s">
         <v>10</v>
       </c>
@@ -884,7 +875,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2">
       <c r="A51" s="4" t="s">
         <v>10</v>
       </c>
@@ -892,7 +883,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2">
       <c r="A52" s="4" t="s">
         <v>10</v>
       </c>
@@ -900,7 +891,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2">
       <c r="A53" s="4" t="s">
         <v>10</v>
       </c>
@@ -908,15 +899,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2">
       <c r="A54" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
       <c r="A55" s="4" t="s">
         <v>10</v>
       </c>
@@ -924,7 +915,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2">
       <c r="A56" s="4" t="s">
         <v>10</v>
       </c>
@@ -932,7 +923,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2">
       <c r="A57" s="4" t="s">
         <v>10</v>
       </c>
@@ -940,7 +931,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2">
       <c r="A58" s="3" t="s">
         <v>12</v>
       </c>
@@ -948,7 +939,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2">
       <c r="A59" s="3" t="s">
         <v>12</v>
       </c>
@@ -956,15 +947,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2">
       <c r="A60" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
       <c r="A61" s="3" t="s">
         <v>12</v>
       </c>
@@ -972,7 +963,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2">
       <c r="A62" s="3" t="s">
         <v>12</v>
       </c>
@@ -980,15 +971,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2">
       <c r="A63" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
       <c r="A64" s="3" t="s">
         <v>12</v>
       </c>
@@ -996,47 +987,47 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2">
       <c r="A65" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
       <c r="A66" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
       <c r="A67" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
       <c r="A68" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
       <c r="A69" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
       <c r="A70" s="3" t="s">
         <v>12</v>
       </c>
@@ -1044,63 +1035,63 @@
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2">
       <c r="A71" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
       <c r="A72" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
       <c r="A73" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
       <c r="A74" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
       <c r="A75" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
       <c r="A76" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
       <c r="A77" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
       <c r="A78" s="3" t="s">
         <v>13</v>
       </c>
@@ -1108,23 +1099,23 @@
         <v>11</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2">
       <c r="A79" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
       <c r="A80" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
       <c r="A81" s="3" t="s">
         <v>13</v>
       </c>
@@ -1132,7 +1123,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2">
       <c r="A82" s="3" t="s">
         <v>13</v>
       </c>
@@ -1140,7 +1131,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2">
       <c r="A83" s="3" t="s">
         <v>13</v>
       </c>
@@ -1148,7 +1139,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2">
       <c r="A84" s="3" t="s">
         <v>13</v>
       </c>
@@ -1156,124 +1147,124 @@
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2">
       <c r="A85" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2">
       <c r="A86" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2">
       <c r="A87" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2">
       <c r="A88" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
       <c r="A89" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2">
       <c r="A90" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2">
       <c r="A91" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
       <c r="A92" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
       <c r="A93" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2">
       <c r="A94" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2">
       <c r="A95" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2">
       <c r="A96" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
       <c r="A97" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
       <c r="A98" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
       <c r="A99" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>